<commit_message>
Added elective in 2021
</commit_message>
<xml_diff>
--- a/edited/elective_list/DBinfo.xlsx
+++ b/edited/elective_list/DBinfo.xlsx
@@ -1,34 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GIST_Credit_Analysis_Program\edited\elective_list\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22693D33-B268-496C-85E1-11D3E6ED188E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>DB Updated Date</t>
+  </si>
+  <si>
+    <t>HUS, PPE Applied Year</t>
+  </si>
+  <si>
+    <t>2021.02.02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -44,83 +70,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,42 +375,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>DB Updated Date</t>
-        </is>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>2021.01.13</t>
-        </is>
+      <c r="B1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>HUS, PPE Applied Year</t>
-        </is>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>2020</v>
+      <c r="B2">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added elective courses and fixed minor
</commit_message>
<xml_diff>
--- a/edited/elective_list/DBinfo.xlsx
+++ b/edited/elective_list/DBinfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GIST_Credit_Analysis_Program\edited\elective_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22693D33-B268-496C-85E1-11D3E6ED188E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C30194-CB16-4DDC-AF53-44533976591B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="2976" windowWidth="11460" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <t>HUS, PPE Applied Year</t>
   </si>
   <si>
-    <t>2021.02.02</t>
+    <t>2021.02.18</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -379,7 +379,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
course bug(elective, MC major) fix
</commit_message>
<xml_diff>
--- a/edited/elective_list/DBinfo.xlsx
+++ b/edited/elective_list/DBinfo.xlsx
@@ -1,60 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GIST_Credit_Analysis_Program\edited\elective_list\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C30194-CB16-4DDC-AF53-44533976591B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="2976" windowWidth="11460" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>DB Updated Date</t>
-  </si>
-  <si>
-    <t>HUS, PPE Applied Year</t>
-  </si>
-  <si>
-    <t>2021.02.18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,24 +44,83 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -375,34 +408,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>DB Updated Date</t>
+        </is>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2021.02.25</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>HUS, PPE Applied Year</t>
+        </is>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>2021</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
elective sort bug fix
</commit_message>
<xml_diff>
--- a/edited/elective_list/DBinfo.xlsx
+++ b/edited/elective_list/DBinfo.xlsx
@@ -1,60 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GIST_Credit_Analysis_Program\edited\elective_list\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F773693D-70EB-43F9-893F-0DB0A488F0B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="9048" yWindow="2448" windowWidth="11460" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>DB Updated Date</t>
-  </si>
-  <si>
-    <t>HUS, PPE Applied Year</t>
-  </si>
-  <si>
-    <t>2021.03.02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,24 +44,83 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -375,34 +408,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>DB Updated Date</t>
+        </is>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>2021.03.02</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>HUS, PPE Applied Year</t>
+        </is>
       </c>
-      <c r="B2">
-        <v>2021</v>
+      <c r="B2" t="n">
+        <v>2016</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>